<commit_message>
Added Characters to Excel
</commit_message>
<xml_diff>
--- a/Character Sheets/Character Sheet.xlsx
+++ b/Character Sheets/Character Sheet.xlsx
@@ -7,15 +7,19 @@
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="OtherTables" sheetId="2" r:id="rId2"/>
+    <sheet name="Martha" sheetId="6" r:id="rId1"/>
+    <sheet name="James" sheetId="5" r:id="rId2"/>
+    <sheet name="Liam" sheetId="4" r:id="rId3"/>
+    <sheet name="Ciara" sheetId="3" r:id="rId4"/>
+    <sheet name="Template" sheetId="1" r:id="rId5"/>
+    <sheet name="OtherTables" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="59">
   <si>
     <t>S</t>
   </si>
@@ -256,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -265,9 +269,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -279,6 +280,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -588,6 +595,402 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="4.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" customWidth="1"/>
+    <col min="8" max="8" width="26" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="F1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="9"/>
+      <c r="J1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4">
+        <f>5+(D7*4)</f>
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2">
+        <f>15+D2 +(2*D4)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4">
+        <f>D7*2</f>
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3">
+        <f>D7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="4">
+        <f>D7*2</f>
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <f>INDEX(OtherTables!E2:E20,MATCH(D7,OtherTables!D2:D20))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4">
+        <f>30+(2*(D7 +D2))</f>
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5">
+        <f>25+(D2*25)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4">
+        <f>20+(2*(D7 +D2))</f>
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6">
+        <f>INDEX(OtherTables!H2:H20,MATCH(D2,OtherTables!G2:G20))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="4">
+        <f>D7*4</f>
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7">
+        <f>2*D3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4">
+        <f>2*(D2+D4)</f>
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8">
+        <f>INDEX(OtherTables!B2:B20,MATCH(D4,OtherTables!A2:A20))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D9" s="2" t="str">
+        <f>CONCATENATE(SUM(D2:D8), "/40")</f>
+        <v>7/40</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="4">
+        <f>5+D3+D6</f>
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9">
+        <f>D8</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="4">
+        <f>5+(D7*3)</f>
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10">
+        <f>3+(D4/2)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="4">
+        <f>10 +D3+D7</f>
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11">
+        <f>5+(D6*2)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="4">
+        <f>D7*3</f>
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="4">
+        <f>10+D3+D7</f>
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="4">
+        <f>D6*4</f>
+        <v>4</v>
+      </c>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="4">
+        <f>D6*3</f>
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="4">
+        <f>2 * (D7 +D3)</f>
+        <v>4</v>
+      </c>
+      <c r="H16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="4">
+        <f>5*D5</f>
+        <v>5</v>
+      </c>
+      <c r="H17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="4">
+        <f>4*D5</f>
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="4">
+        <f>5*D8</f>
+        <v>5</v>
+      </c>
+      <c r="H19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="5">
+        <f>2*(D4+D6)</f>
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F22" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
@@ -602,33 +1005,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="D1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="G1" s="9"/>
+      <c r="J1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="4"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <f>5+(D7*4)</f>
         <v>9</v>
       </c>
@@ -644,16 +1047,16 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <f>D7*2</f>
         <v>2</v>
       </c>
@@ -669,19 +1072,19 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <f>D7*2</f>
         <v>2</v>
       </c>
@@ -697,16 +1100,16 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <f>30+(2*(D7 +D2))</f>
         <v>34</v>
       </c>
@@ -722,16 +1125,16 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <f>20+(2*(D7 +D2))</f>
         <v>24</v>
       </c>
@@ -747,16 +1150,16 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <f>D7*4</f>
         <v>4</v>
       </c>
@@ -772,16 +1175,16 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <f>2*(D2+D4)</f>
         <v>4</v>
       </c>
@@ -801,10 +1204,10 @@
         <f>CONCATENATE(SUM(D2:D8), "/40")</f>
         <v>7/40</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <f>5+D3+D6</f>
         <v>7</v>
       </c>
@@ -820,10 +1223,10 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <f>5+(D7*3)</f>
         <v>8</v>
       </c>
@@ -839,10 +1242,10 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <f>10 +D3+D7</f>
         <v>12</v>
       </c>
@@ -858,10 +1261,10 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <f>D7*3</f>
         <v>3</v>
       </c>
@@ -870,10 +1273,10 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <f>10+D3+D7</f>
         <v>12</v>
       </c>
@@ -882,10 +1285,10 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <f>D6*4</f>
         <v>4</v>
       </c>
@@ -894,10 +1297,10 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <f>D6*3</f>
         <v>3</v>
       </c>
@@ -906,10 +1309,10 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <f>2 * (D7 +D3)</f>
         <v>4</v>
       </c>
@@ -918,10 +1321,10 @@
       </c>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <f>5*D5</f>
         <v>5</v>
       </c>
@@ -930,10 +1333,10 @@
       </c>
     </row>
     <row r="18" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <f>4*D5</f>
         <v>4</v>
       </c>
@@ -942,10 +1345,10 @@
       </c>
     </row>
     <row r="19" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <f>5*D8</f>
         <v>5</v>
       </c>
@@ -954,10 +1357,10 @@
       </c>
     </row>
     <row r="20" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <f>2*(D4+D6)</f>
         <v>4</v>
       </c>
@@ -966,7 +1369,7 @@
       </c>
     </row>
     <row r="22" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F22" s="5"/>
+      <c r="F22" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -979,7 +1382,1195 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="4.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" customWidth="1"/>
+    <col min="8" max="8" width="26" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="F1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="9"/>
+      <c r="J1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4">
+        <f>5+(D7*4)</f>
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2">
+        <f>15+D2 +(2*D4)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4">
+        <f>D7*2</f>
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3">
+        <f>D7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="4">
+        <f>D7*2</f>
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <f>INDEX(OtherTables!E2:E20,MATCH(D7,OtherTables!D2:D20))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4">
+        <f>30+(2*(D7 +D2))</f>
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5">
+        <f>25+(D2*25)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4">
+        <f>20+(2*(D7 +D2))</f>
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6">
+        <f>INDEX(OtherTables!H2:H20,MATCH(D2,OtherTables!G2:G20))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="4">
+        <f>D7*4</f>
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7">
+        <f>2*D3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4">
+        <f>2*(D2+D4)</f>
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8">
+        <f>INDEX(OtherTables!B2:B20,MATCH(D4,OtherTables!A2:A20))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D9" s="2" t="str">
+        <f>CONCATENATE(SUM(D2:D8), "/40")</f>
+        <v>7/40</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="4">
+        <f>5+D3+D6</f>
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9">
+        <f>D8</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="4">
+        <f>5+(D7*3)</f>
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10">
+        <f>3+(D4/2)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="4">
+        <f>10 +D3+D7</f>
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11">
+        <f>5+(D6*2)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="4">
+        <f>D7*3</f>
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="4">
+        <f>10+D3+D7</f>
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="4">
+        <f>D6*4</f>
+        <v>4</v>
+      </c>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="4">
+        <f>D6*3</f>
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="4">
+        <f>2 * (D7 +D3)</f>
+        <v>4</v>
+      </c>
+      <c r="H16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="4">
+        <f>5*D5</f>
+        <v>5</v>
+      </c>
+      <c r="H17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="4">
+        <f>4*D5</f>
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="4">
+        <f>5*D8</f>
+        <v>5</v>
+      </c>
+      <c r="H19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="5">
+        <f>2*(D4+D6)</f>
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F22" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="4.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" customWidth="1"/>
+    <col min="8" max="8" width="26" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="F1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="9"/>
+      <c r="J1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4">
+        <f>5+(D7*4)</f>
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2">
+        <f>15+D2 +(2*D4)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4">
+        <f>D7*2</f>
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3">
+        <f>D7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="4">
+        <f>D7*2</f>
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <f>INDEX(OtherTables!E2:E20,MATCH(D7,OtherTables!D2:D20))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4">
+        <f>30+(2*(D7 +D2))</f>
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5">
+        <f>25+(D2*25)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4">
+        <f>20+(2*(D7 +D2))</f>
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6">
+        <f>INDEX(OtherTables!H2:H20,MATCH(D2,OtherTables!G2:G20))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="4">
+        <f>D7*4</f>
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7">
+        <f>2*D3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4">
+        <f>2*(D2+D4)</f>
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8">
+        <f>INDEX(OtherTables!B2:B20,MATCH(D4,OtherTables!A2:A20))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D9" s="2" t="str">
+        <f>CONCATENATE(SUM(D2:D8), "/40")</f>
+        <v>7/40</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="4">
+        <f>5+D3+D6</f>
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9">
+        <f>D8</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="4">
+        <f>5+(D7*3)</f>
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10">
+        <f>3+(D4/2)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="4">
+        <f>10 +D3+D7</f>
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11">
+        <f>5+(D6*2)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="4">
+        <f>D7*3</f>
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="4">
+        <f>10+D3+D7</f>
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="4">
+        <f>D6*4</f>
+        <v>4</v>
+      </c>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="4">
+        <f>D6*3</f>
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="4">
+        <f>2 * (D7 +D3)</f>
+        <v>4</v>
+      </c>
+      <c r="H16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="4">
+        <f>5*D5</f>
+        <v>5</v>
+      </c>
+      <c r="H17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="4">
+        <f>4*D5</f>
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="4">
+        <f>5*D8</f>
+        <v>5</v>
+      </c>
+      <c r="H19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="5">
+        <f>2*(D4+D6)</f>
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F22" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="4.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" customWidth="1"/>
+    <col min="8" max="8" width="26" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="F1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="9"/>
+      <c r="J1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4">
+        <f>5+(D7*4)</f>
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2">
+        <f>15+D2 +(2*D4)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4">
+        <f>D7*2</f>
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3">
+        <f>D7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="4">
+        <f>D7*2</f>
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <f>INDEX(OtherTables!E2:E20,MATCH(D7,OtherTables!D2:D20))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4">
+        <f>30+(2*(D7 +D2))</f>
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5">
+        <f>25+(D2*25)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4">
+        <f>20+(2*(D7 +D2))</f>
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6">
+        <f>INDEX(OtherTables!H2:H20,MATCH(D2,OtherTables!G2:G20))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="4">
+        <f>D7*4</f>
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7">
+        <f>2*D3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4">
+        <f>2*(D2+D4)</f>
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8">
+        <f>INDEX(OtherTables!B2:B20,MATCH(D4,OtherTables!A2:A20))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D9" s="2" t="str">
+        <f>CONCATENATE(SUM(D2:D8), "/40")</f>
+        <v>7/40</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="4">
+        <f>5+D3+D6</f>
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9">
+        <f>D8</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="4">
+        <f>5+(D7*3)</f>
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10">
+        <f>3+(D4/2)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="4">
+        <f>10 +D3+D7</f>
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11">
+        <f>5+(D6*2)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="4">
+        <f>D7*3</f>
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="4">
+        <f>10+D3+D7</f>
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="4">
+        <f>D6*4</f>
+        <v>4</v>
+      </c>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="4">
+        <f>D6*3</f>
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="4">
+        <f>2 * (D7 +D3)</f>
+        <v>4</v>
+      </c>
+      <c r="H16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="4">
+        <f>5*D5</f>
+        <v>5</v>
+      </c>
+      <c r="H17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="4">
+        <f>4*D5</f>
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="4">
+        <f>5*D8</f>
+        <v>5</v>
+      </c>
+      <c r="H19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="5">
+        <f>2*(D4+D6)</f>
+        <v>4</v>
+      </c>
+      <c r="H20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F22" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
@@ -994,18 +2585,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="E1" s="10"/>
+      <c r="G1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="3"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">

</xml_diff>